<commit_message>
Forgot password and otp api Basic added
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/ScreenList.xlsx
+++ b/Documents/ScreenLayouts/ScreenList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41143A3-CEEB-3649-865A-E7FB90CB17BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033F9644-F50B-EB4E-A31E-62E516F7801F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{D19396D0-D678-A34E-8388-CDC2E3063764}"/>
   </bookViews>
@@ -538,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F49D32-CE35-E740-8DEE-A773068A13AE}">
-  <dimension ref="B3:L24"/>
+  <dimension ref="B3:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +554,7 @@
     <col min="6" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -600,7 +600,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -620,7 +620,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -640,7 +640,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -679,11 +679,8 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="L8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -699,7 +696,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -715,7 +712,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
@@ -735,7 +732,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -755,7 +752,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -775,7 +772,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
@@ -793,7 +790,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
@@ -811,7 +808,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Login Screen changes and Account type display, Home page service
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/ScreenList.xlsx
+++ b/Documents/ScreenLayouts/ScreenList.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D800ED-AD34-DB49-B5DB-BC826EC575A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E60A4B-0C1B-9740-959A-0445406CAE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{D19396D0-D678-A34E-8388-CDC2E3063764}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D19396D0-D678-A34E-8388-CDC2E3063764}"/>
   </bookViews>
   <sheets>
     <sheet name="ScreenList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScreenList!$B$3:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScreenList!$B$3:$I$27</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Service area Add/update/delete</t>
   </si>
   <si>
-    <t>Deepak</t>
-  </si>
-  <si>
     <t>Ravi</t>
   </si>
   <si>
@@ -196,6 +193,21 @@
   </si>
   <si>
     <t>MP</t>
+  </si>
+  <si>
+    <t>Deepak/Atul</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Drawer</t>
+  </si>
+  <si>
+    <t>Ravi/Atul</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -225,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +247,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,13 +290,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -589,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F49D32-CE35-E740-8DEE-A773068A13AE}">
-  <dimension ref="B3:J26"/>
+  <dimension ref="B3:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +633,7 @@
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,49 +664,53 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="4"/>
       <c r="J4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -698,24 +734,29 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -738,49 +779,53 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="6"/>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -804,57 +849,62 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
@@ -871,14 +921,14 @@
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
@@ -891,122 +941,137 @@
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1016,7 +1081,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1026,7 +1091,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1036,7 +1101,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1046,8 +1111,18 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B3:I26" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:I27" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Basic Version Of Profile Screen.
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/ScreenList.xlsx
+++ b/Documents/ScreenLayouts/ScreenList.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E60A4B-0C1B-9740-959A-0445406CAE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9809C535-A717-F84F-8562-895A89B7ED22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D19396D0-D678-A34E-8388-CDC2E3063764}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{D19396D0-D678-A34E-8388-CDC2E3063764}"/>
   </bookViews>
   <sheets>
     <sheet name="ScreenList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScreenList!$B$3:$I$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScreenList!$B$3:$I$28</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Type</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>SCR-CMN-09</t>
   </si>
 </sst>
 </file>
@@ -621,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F49D32-CE35-E740-8DEE-A773068A13AE}">
-  <dimension ref="B3:J27"/>
+  <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,59 +878,59 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
@@ -941,14 +947,14 @@
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>12</v>
@@ -961,16 +967,18 @@
         <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
@@ -979,14 +987,14 @@
         <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
@@ -994,89 +1002,97 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="6" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" t="s">
+      <c r="I21" s="6"/>
+      <c r="J21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1121,8 +1137,18 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B3:I27" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:I28" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>